<commit_message>
added 3v3 5 and 7v power rails
</commit_message>
<xml_diff>
--- a/H2-Sensor-Board2022_Lucy/H2 Sensor Board Lucy Rev 1/BOM.xlsx
+++ b/H2-Sensor-Board2022_Lucy/H2 Sensor Board Lucy Rev 1/BOM.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26731"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26626"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://ualbertaca-my.sharepoint.com/personal/abinash1_ualberta_ca/Documents/Desktop/side/EcoCar/H2 sensor board/H2-Sensor-Board2022_Lucy/H2 Sensor Board Lucy Rev 1/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="16" documentId="11_F25DC773A252ABDACC104874091948605ADE58EE" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{188ED57C-4D95-47E2-AB5A-8BABC842796B}"/>
+  <xr:revisionPtr revIDLastSave="17" documentId="11_F25DC773A252ABDACC104874091948605ADE58EE" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{C49752C4-D4F6-4EF2-BF23-C7CEC8CD337E}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="4260" yWindow="0" windowWidth="21600" windowHeight="11535" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -52,10 +52,18 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -78,13 +86,16 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -370,7 +381,7 @@
   <dimension ref="A3:C5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+      <selection activeCell="J11" sqref="J11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -398,11 +409,14 @@
       <c r="A5" t="s">
         <v>4</v>
       </c>
-      <c r="B5" t="s">
+      <c r="B5" s="1" t="s">
         <v>5</v>
       </c>
     </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="B5" r:id="rId1" xr:uid="{FAB4C3FB-185F-44D6-9571-0C635ED9BB7C}"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Completed Power supply schmatic still have to figure out current limit and install potentiometer, and verify buck
</commit_message>
<xml_diff>
--- a/H2-Sensor-Board2022_Lucy/H2 Sensor Board Lucy Rev 1/BOM.xlsx
+++ b/H2-Sensor-Board2022_Lucy/H2 Sensor Board Lucy Rev 1/BOM.xlsx
@@ -8,17 +8,28 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://ualbertaca-my.sharepoint.com/personal/abinash1_ualberta_ca/Documents/Desktop/side/EcoCar/H2 sensor board/H2-Sensor-Board2022_Lucy/H2 Sensor Board Lucy Rev 1/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="17" documentId="11_F25DC773A252ABDACC104874091948605ADE58EE" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{C49752C4-D4F6-4EF2-BF23-C7CEC8CD337E}"/>
+  <xr:revisionPtr revIDLastSave="19" documentId="11_F25DC773A252ABDACC104874091948605ADE58EE" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{96BE9E7F-6FC7-412F-9EDA-3684F1049B40}"/>
   <bookViews>
-    <workbookView xWindow="4260" yWindow="0" windowWidth="21600" windowHeight="11535" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView minimized="1" xWindow="-13335" yWindow="2310" windowWidth="21600" windowHeight="11535" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
@@ -381,7 +392,7 @@
   <dimension ref="A3:C5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J11" sqref="J11"/>
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -390,10 +401,10 @@
       <c r="A3" t="s">
         <v>3</v>
       </c>
-      <c r="B3" t="s">
+      <c r="B3" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C3" t="s">
+      <c r="C3" s="1" t="s">
         <v>2</v>
       </c>
     </row>
@@ -416,6 +427,8 @@
   </sheetData>
   <hyperlinks>
     <hyperlink ref="B5" r:id="rId1" xr:uid="{FAB4C3FB-185F-44D6-9571-0C635ED9BB7C}"/>
+    <hyperlink ref="C3" r:id="rId2" display="https://www.ti.com/lit/ds/symlink/tps2596.pdf?HQS=dis-dk-null-digikeymode-dsf-pf-null-wwe&amp;ts=1692910049883&amp;ref_url=https%253A%252F%252Fwww.ti.com%252Fgeneral%252Fdocs%252Fsuppproductinfo.tsp%253FdistId%253D10%2526gotoUrl%253Dhttps%253A%252F%252Fwww.ti.com%252Flit%252Fgpn%252Ftps2596" xr:uid="{FF150DED-5690-42E8-94C4-D1C6E5973775}"/>
+    <hyperlink ref="B3" r:id="rId3" xr:uid="{6905841B-67D4-48AD-B04D-D2E1061FBB49}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>